<commit_message>
Preliminary completion of Excel tool.
</commit_message>
<xml_diff>
--- a/office/example/result.xlsx
+++ b/office/example/result.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>{{xxx}}</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -37,6 +37,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>{{.nieaowei}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>nieaowei</t>
   </si>
   <si>
@@ -50,6 +54,21 @@
   </si>
   <si>
     <t>dioasdoihasd</t>
+  </si>
+  <si>
+    <t>dsadsa</t>
+  </si>
+  <si>
+    <t>1231313</t>
+  </si>
+  <si>
+    <t>dsadqweqeasd</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>fyw是傻逼</t>
   </si>
 </sst>
 </file>
@@ -428,7 +447,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B9"/>
+      <selection activeCell="F4" sqref="F4:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -445,31 +464,31 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" t="s">
-        <v>4</v>
-      </c>
       <c r="Q1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -485,13 +504,13 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -507,13 +526,13 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -528,22 +547,22 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" t="s">
         <v>5</v>
       </c>
-      <c r="P4" t="s">
-        <v>4</v>
-      </c>
       <c r="Q4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -574,11 +593,15 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -586,22 +609,22 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -632,7 +655,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -644,7 +667,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -652,18 +675,20 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -716,6 +741,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="G1:J3"/>
+    <mergeCell ref="G4:J6"/>
+    <mergeCell ref="G7:J9"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="F4:F6"/>
     <mergeCell ref="F7:F9"/>
@@ -729,12 +760,6 @@
     <mergeCell ref="D7:E9"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="D1:E3"/>
-    <mergeCell ref="K1:K3"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="G1:J3"/>
-    <mergeCell ref="G4:J6"/>
-    <mergeCell ref="G7:J9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>